<commit_message>
Connected MACE isomers to ChemSpaX functionalization, updated the relevant test files.
</commit_message>
<xml_diff>
--- a/obelix/demo_chemspax_cv.xlsx
+++ b/obelix/demo_chemspax_cv.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -407,7 +407,7 @@
         <v>Name</v>
       </c>
       <c r="B1" t="str">
-        <v>Skeleton</v>
+        <v>Functionalization</v>
       </c>
       <c r="C1" t="str">
         <v>R1</v>
@@ -424,47 +424,87 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>96183-46-9</v>
+        <v>skeleton_1</v>
       </c>
       <c r="B2" t="str">
-        <v>[Ir+3]_96183-46-9_SP0.xyz</v>
+        <v>1</v>
       </c>
       <c r="C2" t="str">
-        <v>C6H6</v>
+        <v>CH3</v>
       </c>
       <c r="D2" t="str">
-        <v>C6H6</v>
+        <v>CH3</v>
       </c>
       <c r="E2" t="str">
-        <v>C6H6</v>
+        <v>CH3</v>
       </c>
       <c r="F2" t="str">
-        <v>C6H6</v>
+        <v>CH3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>96183-46-9_</v>
+        <v>skeleton_1</v>
       </c>
       <c r="B3" t="str">
-        <v>[Ir+3]_96183-46-9_SP1.xyz</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
-        <v>C6H6</v>
+        <v>CCH3CH3CH3</v>
       </c>
       <c r="D3" t="str">
-        <v>C6H6</v>
+        <v>CCH3CH3CH3</v>
       </c>
       <c r="E3" t="str">
-        <v>C6H6</v>
+        <v>CCH3CH3CH3</v>
       </c>
       <c r="F3" t="str">
-        <v>C6H6</v>
+        <v>CCH3CH3CH3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>skeleton_2</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>CH3</v>
+      </c>
+      <c r="D4" t="str">
+        <v>CH3</v>
+      </c>
+      <c r="E4" t="str">
+        <v>CH3</v>
+      </c>
+      <c r="F4" t="str">
+        <v>CH3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>skeleton_2</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2</v>
+      </c>
+      <c r="C5" t="str">
+        <v>CCH3CH3CH3</v>
+      </c>
+      <c r="D5" t="str">
+        <v>CCH3CH3CH3</v>
+      </c>
+      <c r="E5" t="str">
+        <v>CCH3CH3CH3</v>
+      </c>
+      <c r="F5" t="str">
+        <v>CCH3CH3CH3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>